<commit_message>
GPS Removed, added back original display, kept pads for adafruit display
</commit_message>
<xml_diff>
--- a/Hardware/Extra/Top/Smartwatch-EXTRA-TOP_BOM.xlsx
+++ b/Hardware/Extra/Top/Smartwatch-EXTRA-TOP_BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ruhaan Joshi\Documents\Smartwatch\Hardware\Extra\Top\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8946529-7FE9-4C9B-B3FD-B3E0E4217ED7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDEFBF51-BC25-40A9-A8BF-ABB32A3E80B5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7290" yWindow="3360" windowWidth="14400" windowHeight="11340" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7635" yWindow="3705" windowWidth="14400" windowHeight="11340" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -236,7 +236,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="245">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="240">
   <si>
     <t>BOM #</t>
   </si>
@@ -424,15 +424,6 @@
     <t>Adafruit Industries LLC</t>
   </si>
   <si>
-    <t xml:space="preserve"> 3.7V Lithium-Ion Battery Rechargeable (Secondary) 350mAh</t>
-  </si>
-  <si>
-    <t>2750</t>
-  </si>
-  <si>
-    <t>1528-1858-ND</t>
-  </si>
-  <si>
     <t>CRYSTALECS-.327-12.5-12-C-TR (CRYSTAL) (32.7680kHz)</t>
   </si>
   <si>
@@ -676,15 +667,6 @@
     <t>1292-1528-1-ND</t>
   </si>
   <si>
-    <t>120pF ±5% 50V Ceramic Capacitor C0G, NP0 0603 (1608 Metric)</t>
-  </si>
-  <si>
-    <t>0603N121J500CT</t>
-  </si>
-  <si>
-    <t>1292-1481-1-ND</t>
-  </si>
-  <si>
     <t>100 nF Capacitor</t>
   </si>
   <si>
@@ -784,18 +766,6 @@
     <t>R3,R4,R15, R16</t>
   </si>
   <si>
-    <t>C2,C7</t>
-  </si>
-  <si>
-    <t>C15,C17</t>
-  </si>
-  <si>
-    <t>C14,C20</t>
-  </si>
-  <si>
-    <t>300 pF Capacitor</t>
-  </si>
-  <si>
     <t>CHRG1</t>
   </si>
   <si>
@@ -877,9 +847,6 @@
     <t>R8,R12,R13,R14</t>
   </si>
   <si>
-    <t>C5,C6</t>
-  </si>
-  <si>
     <t>U5</t>
   </si>
   <si>
@@ -910,18 +877,6 @@
     <t>C3,C4</t>
   </si>
   <si>
-    <t>C8,C9,C10,C11,C12,C21</t>
-  </si>
-  <si>
-    <t>C23</t>
-  </si>
-  <si>
-    <t>C1,C16,C19,C24</t>
-  </si>
-  <si>
-    <t>C13,C18,C22,C25</t>
-  </si>
-  <si>
     <t>NFET</t>
   </si>
   <si>
@@ -971,6 +926,36 @@
   </si>
   <si>
     <t>R6</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 3.7V Lithium Polymer Battery Rechargeable (Secondary) 350mAh</t>
+  </si>
+  <si>
+    <t>4237</t>
+  </si>
+  <si>
+    <t>1528-4237-ND</t>
+  </si>
+  <si>
+    <t>C1,C8,C11,C16</t>
+  </si>
+  <si>
+    <t>C13,C18,C19,C21,C22,C23</t>
+  </si>
+  <si>
+    <t>C6, C12</t>
+  </si>
+  <si>
+    <t>C15</t>
+  </si>
+  <si>
+    <t>C2,C20</t>
+  </si>
+  <si>
+    <t>C7, C9</t>
+  </si>
+  <si>
+    <t>C5,C10,C14,C17</t>
   </si>
 </sst>
 </file>
@@ -1293,7 +1278,7 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1389,6 +1374,11 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="84" applyFont="1"/>
+    <xf numFmtId="44" fontId="11" fillId="0" borderId="0" xfId="84" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="84" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="84" applyFont="1"/>
+    <xf numFmtId="44" fontId="14" fillId="0" borderId="0" xfId="84" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="85">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1812,10 +1802,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z43"/>
+  <dimension ref="A1:Z42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="11.25"/>
@@ -1853,15 +1843,15 @@
         <v>13</v>
       </c>
       <c r="M1" s="6">
-        <f>SUM(M3:M22)</f>
-        <v>39.468999999999994</v>
+        <f>SUM(M3:M21)</f>
+        <v>32.518999999999998</v>
       </c>
       <c r="N1" s="5" t="s">
         <v>29</v>
       </c>
       <c r="O1" s="6">
-        <f>SUM(O3:O22)</f>
-        <v>34.247299999999996</v>
+        <f>SUM(O3:O21)</f>
+        <v>27.297300000000003</v>
       </c>
     </row>
     <row r="2" spans="1:26" s="2" customFormat="1" ht="10.5">
@@ -1977,7 +1967,7 @@
         <v>34</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>189</v>
+        <v>179</v>
       </c>
       <c r="D5" s="18" t="s">
         <v>35</v>
@@ -2019,7 +2009,7 @@
         <v>10.1</v>
       </c>
       <c r="P5" s="13" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="Q5" s="12"/>
       <c r="R5" s="12"/>
@@ -2041,7 +2031,7 @@
         <v>40</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>191</v>
+        <v>181</v>
       </c>
       <c r="D6" s="18" t="s">
         <v>41</v>
@@ -2071,18 +2061,18 @@
         <v>1</v>
       </c>
       <c r="M6" s="51">
-        <f t="shared" ref="M6:N43" si="0">L6*K6</f>
+        <f t="shared" ref="M6:N41" si="0">L6*K6</f>
         <v>2.12</v>
       </c>
       <c r="N6" s="51">
         <v>2.08</v>
       </c>
       <c r="O6" s="51">
-        <f t="shared" ref="O6:O43" si="1">N6*L6</f>
+        <f t="shared" ref="O6:O41" si="1">N6*L6</f>
         <v>2.08</v>
       </c>
       <c r="P6" s="13" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="Q6" s="12"/>
       <c r="R6" s="12"/>
@@ -2097,56 +2087,55 @@
     </row>
     <row r="7" spans="1:26">
       <c r="A7" s="49">
-        <f t="shared" ref="A7:A43" si="2">A6+1</f>
+        <f t="shared" ref="A7:A42" si="2">A6+1</f>
         <v>3</v>
       </c>
-      <c r="B7" s="13" t="s">
-        <v>58</v>
+      <c r="B7" s="18" t="s">
+        <v>46</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>190</v>
-      </c>
-      <c r="D7" s="20" t="s">
-        <v>62</v>
-      </c>
-      <c r="E7" s="20" t="s">
-        <v>59</v>
-      </c>
-      <c r="F7" s="20" t="s">
-        <v>60</v>
-      </c>
-      <c r="G7" s="20" t="s">
-        <v>61</v>
-      </c>
-      <c r="H7" s="20" t="s">
-        <v>63</v>
-      </c>
-      <c r="I7" s="21" t="s">
+        <v>177</v>
+      </c>
+      <c r="D7" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="E7" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="G7" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="H7" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="I7" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="J7" s="20" t="s">
-        <v>64</v>
-      </c>
-      <c r="K7" s="22">
-        <v>6.95</v>
+      <c r="J7" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="K7" s="19">
+        <v>0.11</v>
       </c>
       <c r="L7" s="13">
         <v>1</v>
       </c>
       <c r="M7" s="51">
         <f t="shared" si="0"/>
-        <v>6.95</v>
+        <v>0.11</v>
       </c>
       <c r="N7" s="51">
-        <f t="shared" si="0"/>
-        <v>6.95</v>
+        <v>0.08</v>
       </c>
       <c r="O7" s="51">
         <f t="shared" si="1"/>
-        <v>6.95</v>
+        <v>0.08</v>
       </c>
       <c r="P7" s="13" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
     </row>
     <row r="8" spans="1:26">
@@ -2154,52 +2143,52 @@
         <f t="shared" si="2"/>
         <v>4</v>
       </c>
-      <c r="B8" s="18" t="s">
-        <v>46</v>
+      <c r="B8" s="13" t="s">
+        <v>52</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>187</v>
-      </c>
-      <c r="D8" s="18" t="s">
-        <v>47</v>
-      </c>
-      <c r="E8" s="18" t="s">
+        <v>176</v>
+      </c>
+      <c r="D8" s="21" t="s">
+        <v>53</v>
+      </c>
+      <c r="E8" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="F8" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="G8" s="18" t="s">
+      <c r="F8" s="23" t="s">
+        <v>54</v>
+      </c>
+      <c r="G8" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="H8" s="18" t="s">
-        <v>50</v>
-      </c>
-      <c r="I8" s="18" t="s">
+      <c r="H8" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="I8" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="J8" s="18" t="s">
-        <v>51</v>
-      </c>
-      <c r="K8" s="19">
-        <v>0.11</v>
+      <c r="J8" s="21" t="s">
+        <v>56</v>
+      </c>
+      <c r="K8" s="22">
+        <v>0.56000000000000005</v>
       </c>
       <c r="L8" s="13">
         <v>1</v>
       </c>
       <c r="M8" s="51">
         <f t="shared" si="0"/>
-        <v>0.11</v>
+        <v>0.56000000000000005</v>
       </c>
       <c r="N8" s="51">
-        <v>0.08</v>
+        <v>0.44</v>
       </c>
       <c r="O8" s="51">
         <f t="shared" si="1"/>
-        <v>0.08</v>
+        <v>0.44</v>
       </c>
       <c r="P8" s="13" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
     </row>
     <row r="9" spans="1:26">
@@ -2207,114 +2196,112 @@
         <f t="shared" si="2"/>
         <v>5</v>
       </c>
-      <c r="B9" s="13" t="s">
-        <v>52</v>
-      </c>
-      <c r="C9" s="13" t="s">
-        <v>186</v>
-      </c>
-      <c r="D9" s="21" t="s">
-        <v>53</v>
-      </c>
-      <c r="E9" s="21" t="s">
+      <c r="B9" s="30" t="s">
+        <v>62</v>
+      </c>
+      <c r="C9" s="29" t="s">
+        <v>178</v>
+      </c>
+      <c r="D9" s="30" t="s">
+        <v>63</v>
+      </c>
+      <c r="E9" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="F9" s="23" t="s">
-        <v>54</v>
-      </c>
-      <c r="G9" s="21" t="s">
-        <v>49</v>
-      </c>
-      <c r="H9" s="21" t="s">
-        <v>55</v>
-      </c>
-      <c r="I9" s="21" t="s">
+      <c r="F9" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="G9" s="30" t="s">
+        <v>65</v>
+      </c>
+      <c r="H9" s="30" t="s">
+        <v>66</v>
+      </c>
+      <c r="I9" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="J9" s="21" t="s">
-        <v>56</v>
-      </c>
-      <c r="K9" s="22">
-        <v>0.56000000000000005</v>
-      </c>
-      <c r="L9" s="13">
+      <c r="J9" s="30" t="s">
+        <v>67</v>
+      </c>
+      <c r="K9" s="31">
+        <v>0.59799999999999998</v>
+      </c>
+      <c r="L9" s="29">
         <v>1</v>
       </c>
       <c r="M9" s="51">
         <f t="shared" si="0"/>
-        <v>0.56000000000000005</v>
+        <v>0.59799999999999998</v>
       </c>
       <c r="N9" s="51">
-        <v>0.44</v>
+        <v>0.54339999999999999</v>
       </c>
       <c r="O9" s="51">
         <f t="shared" si="1"/>
-        <v>0.44</v>
-      </c>
-      <c r="P9" s="13" t="s">
-        <v>174</v>
-      </c>
+        <v>0.54339999999999999</v>
+      </c>
+      <c r="P9" s="29"/>
+      <c r="Q9" s="29"/>
+      <c r="R9" s="29"/>
+      <c r="S9" s="29"/>
+      <c r="T9" s="29"/>
+      <c r="U9" s="29"/>
+      <c r="V9" s="29"/>
+      <c r="W9" s="29"/>
+      <c r="X9" s="29"/>
+      <c r="Y9" s="29"/>
+      <c r="Z9" s="29"/>
     </row>
     <row r="10" spans="1:26">
       <c r="A10" s="49">
         <f t="shared" si="2"/>
         <v>6</v>
       </c>
-      <c r="B10" s="30" t="s">
-        <v>65</v>
-      </c>
-      <c r="C10" s="29" t="s">
-        <v>188</v>
-      </c>
-      <c r="D10" s="30" t="s">
-        <v>66</v>
-      </c>
-      <c r="E10" s="30" t="s">
-        <v>12</v>
-      </c>
-      <c r="F10" s="30" t="s">
-        <v>67</v>
-      </c>
-      <c r="G10" s="30" t="s">
+      <c r="B10" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="H10" s="30" t="s">
+      <c r="C10" s="13" t="s">
+        <v>227</v>
+      </c>
+      <c r="D10" s="18" t="s">
         <v>69</v>
       </c>
-      <c r="I10" s="30" t="s">
+      <c r="E10" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="F10" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="G10" s="18" t="s">
+        <v>71</v>
+      </c>
+      <c r="H10" s="18" t="s">
+        <v>72</v>
+      </c>
+      <c r="I10" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="J10" s="30" t="s">
-        <v>70</v>
-      </c>
-      <c r="K10" s="31">
-        <v>0.59799999999999998</v>
-      </c>
-      <c r="L10" s="29">
+      <c r="J10" s="18" t="s">
+        <v>73</v>
+      </c>
+      <c r="K10" s="25">
+        <v>0.69</v>
+      </c>
+      <c r="L10" s="13">
         <v>1</v>
       </c>
       <c r="M10" s="51">
         <f t="shared" si="0"/>
-        <v>0.59799999999999998</v>
+        <v>0.69</v>
       </c>
       <c r="N10" s="51">
-        <v>0.54339999999999999</v>
+        <v>0.52890000000000004</v>
       </c>
       <c r="O10" s="51">
         <f t="shared" si="1"/>
-        <v>0.54339999999999999</v>
-      </c>
-      <c r="P10" s="29"/>
-      <c r="Q10" s="29"/>
-      <c r="R10" s="29"/>
-      <c r="S10" s="29"/>
-      <c r="T10" s="29"/>
-      <c r="U10" s="29"/>
-      <c r="V10" s="29"/>
-      <c r="W10" s="29"/>
-      <c r="X10" s="29"/>
-      <c r="Y10" s="29"/>
-      <c r="Z10" s="29"/>
+        <v>0.52890000000000004</v>
+      </c>
+      <c r="P10" s="13"/>
     </row>
     <row r="11" spans="1:26">
       <c r="A11" s="49">
@@ -2322,48 +2309,48 @@
         <v>7</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="C11" s="13" t="s">
-        <v>242</v>
+        <v>222</v>
       </c>
       <c r="D11" s="18" t="s">
-        <v>72</v>
-      </c>
-      <c r="E11" s="18" t="s">
-        <v>24</v>
-      </c>
-      <c r="F11" s="18" t="s">
-        <v>73</v>
+        <v>75</v>
+      </c>
+      <c r="E11" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="F11" s="24" t="s">
+        <v>76</v>
       </c>
       <c r="G11" s="18" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="H11" s="18" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="I11" s="18" t="s">
         <v>9</v>
       </c>
       <c r="J11" s="18" t="s">
-        <v>76</v>
-      </c>
-      <c r="K11" s="25">
-        <v>0.69</v>
+        <v>79</v>
+      </c>
+      <c r="K11" s="19">
+        <v>0.25600000000000001</v>
       </c>
       <c r="L11" s="13">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="M11" s="51">
         <f t="shared" si="0"/>
-        <v>0.69</v>
+        <v>1.28</v>
       </c>
       <c r="N11" s="51">
-        <v>0.52890000000000004</v>
+        <v>0.12889999999999999</v>
       </c>
       <c r="O11" s="51">
         <f t="shared" si="1"/>
-        <v>0.52890000000000004</v>
+        <v>0.64449999999999996</v>
       </c>
       <c r="P11" s="13"/>
     </row>
@@ -2373,48 +2360,48 @@
         <v>8</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="C12" s="13" t="s">
-        <v>237</v>
-      </c>
-      <c r="D12" s="18" t="s">
-        <v>78</v>
-      </c>
-      <c r="E12" s="13" t="s">
+        <v>170</v>
+      </c>
+      <c r="D12" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="E12" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="F12" s="24" t="s">
-        <v>79</v>
-      </c>
-      <c r="G12" s="18" t="s">
-        <v>80</v>
-      </c>
-      <c r="H12" s="18" t="s">
-        <v>81</v>
+      <c r="F12" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="G12" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="H12" s="13" t="s">
+        <v>83</v>
       </c>
       <c r="I12" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="J12" s="18" t="s">
-        <v>82</v>
+      <c r="J12" s="13" t="s">
+        <v>84</v>
       </c>
       <c r="K12" s="19">
-        <v>0.25600000000000001</v>
+        <v>0.17699999999999999</v>
       </c>
       <c r="L12" s="13">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="M12" s="51">
         <f t="shared" si="0"/>
-        <v>1.28</v>
+        <v>0.35399999999999998</v>
       </c>
       <c r="N12" s="51">
-        <v>0.12889999999999999</v>
+        <v>8.6099999999999996E-2</v>
       </c>
       <c r="O12" s="51">
         <f t="shared" si="1"/>
-        <v>0.64449999999999996</v>
+        <v>0.17219999999999999</v>
       </c>
       <c r="P12" s="13"/>
     </row>
@@ -2424,13 +2411,13 @@
         <v>9</v>
       </c>
       <c r="B13" s="13" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="C13" s="13" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="D13" s="13" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="E13" s="18" t="s">
         <v>12</v>
@@ -2439,33 +2426,33 @@
         <v>15</v>
       </c>
       <c r="G13" s="13" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="H13" s="13" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="I13" s="18" t="s">
         <v>9</v>
       </c>
       <c r="J13" s="13" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="K13" s="19">
         <v>0.17699999999999999</v>
       </c>
       <c r="L13" s="13">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M13" s="51">
         <f t="shared" si="0"/>
-        <v>0.35399999999999998</v>
+        <v>0.17699999999999999</v>
       </c>
       <c r="N13" s="51">
         <v>8.6099999999999996E-2</v>
       </c>
       <c r="O13" s="51">
         <f t="shared" si="1"/>
-        <v>0.17219999999999999</v>
+        <v>8.6099999999999996E-2</v>
       </c>
       <c r="P13" s="13"/>
     </row>
@@ -2475,13 +2462,13 @@
         <v>10</v>
       </c>
       <c r="B14" s="13" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C14" s="13" t="s">
-        <v>177</v>
-      </c>
-      <c r="D14" s="13" t="s">
-        <v>89</v>
+        <v>172</v>
+      </c>
+      <c r="D14" s="18" t="s">
+        <v>90</v>
       </c>
       <c r="E14" s="18" t="s">
         <v>12</v>
@@ -2489,34 +2476,34 @@
       <c r="F14" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="G14" s="13" t="s">
-        <v>85</v>
-      </c>
-      <c r="H14" s="13" t="s">
-        <v>90</v>
+      <c r="G14" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="H14" s="18" t="s">
+        <v>92</v>
       </c>
       <c r="I14" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="J14" s="13" t="s">
-        <v>91</v>
+      <c r="J14" s="18" t="s">
+        <v>93</v>
       </c>
       <c r="K14" s="19">
-        <v>0.17699999999999999</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="L14" s="13">
         <v>1</v>
       </c>
       <c r="M14" s="51">
         <f t="shared" si="0"/>
-        <v>0.17699999999999999</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="N14" s="51">
-        <v>8.6099999999999996E-2</v>
+        <v>0.114</v>
       </c>
       <c r="O14" s="51">
         <f t="shared" si="1"/>
-        <v>8.6099999999999996E-2</v>
+        <v>0.114</v>
       </c>
       <c r="P14" s="13"/>
     </row>
@@ -2525,332 +2512,330 @@
         <f t="shared" si="2"/>
         <v>11</v>
       </c>
-      <c r="B15" s="13" t="s">
-        <v>92</v>
-      </c>
-      <c r="C15" s="13" t="s">
-        <v>178</v>
-      </c>
-      <c r="D15" s="18" t="s">
-        <v>93</v>
-      </c>
-      <c r="E15" s="18" t="s">
+      <c r="B15" s="36" t="s">
+        <v>182</v>
+      </c>
+      <c r="C15" s="35" t="s">
+        <v>169</v>
+      </c>
+      <c r="D15" s="36" t="s">
+        <v>183</v>
+      </c>
+      <c r="E15" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="F15" s="18" t="s">
+      <c r="F15" s="36" t="s">
         <v>15</v>
       </c>
-      <c r="G15" s="18" t="s">
-        <v>94</v>
-      </c>
-      <c r="H15" s="18" t="s">
-        <v>95</v>
-      </c>
-      <c r="I15" s="18" t="s">
+      <c r="G15" s="36" t="s">
+        <v>82</v>
+      </c>
+      <c r="H15" s="36" t="s">
+        <v>184</v>
+      </c>
+      <c r="I15" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="J15" s="18" t="s">
-        <v>96</v>
-      </c>
-      <c r="K15" s="19">
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="L15" s="13">
+      <c r="J15" s="36" t="s">
+        <v>185</v>
+      </c>
+      <c r="K15" s="37">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="L15" s="35">
         <v>1</v>
       </c>
       <c r="M15" s="51">
         <f t="shared" si="0"/>
-        <v>0.14000000000000001</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="N15" s="51">
-        <v>0.114</v>
+        <v>0.2586</v>
       </c>
       <c r="O15" s="51">
         <f t="shared" si="1"/>
-        <v>0.114</v>
-      </c>
-      <c r="P15" s="13"/>
-    </row>
-    <row r="16" spans="1:26">
+        <v>0.2586</v>
+      </c>
+      <c r="P15" s="35"/>
+      <c r="Q15" s="35"/>
+      <c r="R15" s="35"/>
+      <c r="S15" s="35"/>
+      <c r="T15" s="35"/>
+      <c r="U15" s="35"/>
+      <c r="V15" s="35"/>
+      <c r="W15" s="35"/>
+      <c r="X15" s="35"/>
+      <c r="Y15" s="35"/>
+      <c r="Z15" s="35"/>
+    </row>
+    <row r="16" spans="1:26" ht="12">
       <c r="A16" s="49">
         <f t="shared" si="2"/>
         <v>12</v>
       </c>
-      <c r="B16" s="36" t="s">
-        <v>192</v>
-      </c>
-      <c r="C16" s="35" t="s">
-        <v>175</v>
-      </c>
-      <c r="D16" s="36" t="s">
-        <v>193</v>
-      </c>
-      <c r="E16" s="36" t="s">
+      <c r="B16" s="35" t="s">
+        <v>186</v>
+      </c>
+      <c r="C16" s="13" t="s">
+        <v>203</v>
+      </c>
+      <c r="D16" s="48" t="s">
+        <v>209</v>
+      </c>
+      <c r="E16" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="F16" s="36" t="s">
-        <v>15</v>
-      </c>
-      <c r="G16" s="36" t="s">
-        <v>85</v>
-      </c>
-      <c r="H16" s="36" t="s">
-        <v>194</v>
-      </c>
-      <c r="I16" s="36" t="s">
+      <c r="F16" s="13"/>
+      <c r="G16" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="H16" s="48" t="s">
+        <v>210</v>
+      </c>
+      <c r="I16" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="J16" s="36" t="s">
-        <v>195</v>
-      </c>
-      <c r="K16" s="37">
-        <v>0.55000000000000004</v>
-      </c>
-      <c r="L16" s="35">
+      <c r="J16" s="52" t="s">
+        <v>211</v>
+      </c>
+      <c r="K16" s="19">
+        <v>1.1299999999999999</v>
+      </c>
+      <c r="L16" s="13">
         <v>1</v>
       </c>
       <c r="M16" s="51">
         <f t="shared" si="0"/>
-        <v>0.55000000000000004</v>
+        <v>1.1299999999999999</v>
       </c>
       <c r="N16" s="51">
-        <v>0.2586</v>
+        <v>0.85</v>
       </c>
       <c r="O16" s="51">
         <f t="shared" si="1"/>
-        <v>0.2586</v>
-      </c>
-      <c r="P16" s="35"/>
-      <c r="Q16" s="35"/>
-      <c r="R16" s="35"/>
-      <c r="S16" s="35"/>
-      <c r="T16" s="35"/>
-      <c r="U16" s="35"/>
-      <c r="V16" s="35"/>
-      <c r="W16" s="35"/>
-      <c r="X16" s="35"/>
-      <c r="Y16" s="35"/>
-      <c r="Z16" s="35"/>
-    </row>
-    <row r="17" spans="1:26" ht="12">
+        <v>0.85</v>
+      </c>
+      <c r="P16" s="13"/>
+    </row>
+    <row r="17" spans="1:26">
       <c r="A17" s="49">
         <f t="shared" si="2"/>
         <v>13</v>
       </c>
-      <c r="B17" s="35" t="s">
-        <v>196</v>
-      </c>
-      <c r="C17" s="13" t="s">
+      <c r="B17" s="54" t="s">
+        <v>213</v>
+      </c>
+      <c r="C17" s="53" t="s">
+        <v>188</v>
+      </c>
+      <c r="D17" s="54" t="s">
         <v>214</v>
       </c>
-      <c r="D17" s="48" t="s">
-        <v>220</v>
-      </c>
-      <c r="E17" s="13" t="s">
+      <c r="E17" s="54" t="s">
         <v>12</v>
       </c>
-      <c r="F17" s="13"/>
-      <c r="G17" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="H17" s="48" t="s">
-        <v>221</v>
-      </c>
-      <c r="I17" s="13" t="s">
+      <c r="F17" s="54" t="s">
+        <v>215</v>
+      </c>
+      <c r="G17" s="54" t="s">
+        <v>216</v>
+      </c>
+      <c r="H17" s="54" t="s">
+        <v>217</v>
+      </c>
+      <c r="I17" s="54" t="s">
         <v>9</v>
       </c>
-      <c r="J17" s="52" t="s">
-        <v>222</v>
-      </c>
-      <c r="K17" s="19">
-        <v>1.1299999999999999</v>
-      </c>
-      <c r="L17" s="13">
+      <c r="J17" s="54" t="s">
+        <v>218</v>
+      </c>
+      <c r="K17" s="55">
+        <v>0.27</v>
+      </c>
+      <c r="L17" s="53">
         <v>1</v>
       </c>
       <c r="M17" s="51">
         <f t="shared" si="0"/>
-        <v>1.1299999999999999</v>
-      </c>
-      <c r="N17" s="51">
-        <v>0.85</v>
+        <v>0.27</v>
+      </c>
+      <c r="N17" s="55">
+        <v>9.1999999999999998E-2</v>
       </c>
       <c r="O17" s="51">
         <f t="shared" si="1"/>
-        <v>0.85</v>
-      </c>
-      <c r="P17" s="13"/>
+        <v>9.1999999999999998E-2</v>
+      </c>
+      <c r="P17" s="53"/>
+      <c r="Q17" s="53"/>
+      <c r="R17" s="53"/>
+      <c r="S17" s="53"/>
+      <c r="T17" s="53"/>
+      <c r="U17" s="53"/>
+      <c r="V17" s="53"/>
+      <c r="W17" s="53"/>
+      <c r="X17" s="53"/>
+      <c r="Y17" s="53"/>
+      <c r="Z17" s="53"/>
     </row>
     <row r="18" spans="1:26">
       <c r="A18" s="49">
         <f t="shared" si="2"/>
         <v>14</v>
       </c>
-      <c r="B18" s="54" t="s">
-        <v>228</v>
-      </c>
-      <c r="C18" s="53" t="s">
-        <v>198</v>
-      </c>
-      <c r="D18" s="54" t="s">
-        <v>229</v>
-      </c>
-      <c r="E18" s="54" t="s">
-        <v>12</v>
-      </c>
-      <c r="F18" s="54" t="s">
-        <v>230</v>
-      </c>
-      <c r="G18" s="54" t="s">
-        <v>231</v>
-      </c>
-      <c r="H18" s="54" t="s">
-        <v>232</v>
-      </c>
-      <c r="I18" s="54" t="s">
+      <c r="B18" s="39" t="s">
+        <v>190</v>
+      </c>
+      <c r="C18" s="38" t="s">
+        <v>189</v>
+      </c>
+      <c r="D18" s="39" t="s">
+        <v>191</v>
+      </c>
+      <c r="E18" s="39" t="s">
+        <v>24</v>
+      </c>
+      <c r="F18" s="39" t="s">
+        <v>192</v>
+      </c>
+      <c r="G18" s="39" t="s">
+        <v>193</v>
+      </c>
+      <c r="H18" s="39" t="s">
+        <v>194</v>
+      </c>
+      <c r="I18" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="J18" s="54" t="s">
-        <v>233</v>
-      </c>
-      <c r="K18" s="55">
-        <v>0.27</v>
-      </c>
-      <c r="L18" s="53">
+      <c r="J18" s="39" t="s">
+        <v>195</v>
+      </c>
+      <c r="K18" s="40">
+        <v>3.54</v>
+      </c>
+      <c r="L18" s="38">
         <v>1</v>
       </c>
       <c r="M18" s="51">
         <f t="shared" si="0"/>
-        <v>0.27</v>
-      </c>
-      <c r="N18" s="55">
-        <v>9.1999999999999998E-2</v>
+        <v>3.54</v>
+      </c>
+      <c r="N18" s="51">
+        <v>2.6082000000000001</v>
       </c>
       <c r="O18" s="51">
         <f t="shared" si="1"/>
-        <v>9.1999999999999998E-2</v>
-      </c>
-      <c r="P18" s="53"/>
-      <c r="Q18" s="53"/>
-      <c r="R18" s="53"/>
-      <c r="S18" s="53"/>
-      <c r="T18" s="53"/>
-      <c r="U18" s="53"/>
-      <c r="V18" s="53"/>
-      <c r="W18" s="53"/>
-      <c r="X18" s="53"/>
-      <c r="Y18" s="53"/>
-      <c r="Z18" s="53"/>
+        <v>2.6082000000000001</v>
+      </c>
+      <c r="P18" s="38"/>
+      <c r="Q18" s="38"/>
+      <c r="R18" s="38"/>
+      <c r="S18" s="38"/>
+      <c r="T18" s="38"/>
+      <c r="U18" s="38"/>
+      <c r="V18" s="38"/>
+      <c r="W18" s="38"/>
+      <c r="X18" s="38"/>
+      <c r="Y18" s="38"/>
+      <c r="Z18" s="38"/>
     </row>
     <row r="19" spans="1:26">
       <c r="A19" s="49">
         <f t="shared" si="2"/>
         <v>15</v>
       </c>
-      <c r="B19" s="39" t="s">
-        <v>200</v>
-      </c>
-      <c r="C19" s="38" t="s">
-        <v>199</v>
-      </c>
-      <c r="D19" s="39" t="s">
-        <v>201</v>
-      </c>
-      <c r="E19" s="39" t="s">
-        <v>24</v>
-      </c>
-      <c r="F19" s="39" t="s">
-        <v>202</v>
-      </c>
-      <c r="G19" s="39" t="s">
-        <v>203</v>
-      </c>
-      <c r="H19" s="39" t="s">
-        <v>204</v>
-      </c>
-      <c r="I19" s="39" t="s">
+      <c r="B19" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="C19" s="13" t="s">
+        <v>174</v>
+      </c>
+      <c r="D19" s="18" t="s">
+        <v>102</v>
+      </c>
+      <c r="E19" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="F19" s="18" t="s">
+        <v>103</v>
+      </c>
+      <c r="G19" s="26" t="s">
+        <v>104</v>
+      </c>
+      <c r="H19" s="18" t="s">
+        <v>105</v>
+      </c>
+      <c r="I19" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="J19" s="39" t="s">
-        <v>205</v>
-      </c>
-      <c r="K19" s="40">
-        <v>3.54</v>
-      </c>
-      <c r="L19" s="38">
+      <c r="J19" s="18" t="s">
+        <v>106</v>
+      </c>
+      <c r="K19" s="19">
+        <v>0.43</v>
+      </c>
+      <c r="L19" s="13">
         <v>1</v>
       </c>
       <c r="M19" s="51">
         <f t="shared" si="0"/>
-        <v>3.54</v>
+        <v>0.43</v>
       </c>
       <c r="N19" s="51">
-        <v>2.6082000000000001</v>
+        <v>0.31580000000000003</v>
       </c>
       <c r="O19" s="51">
         <f t="shared" si="1"/>
-        <v>2.6082000000000001</v>
-      </c>
-      <c r="P19" s="38"/>
-      <c r="Q19" s="38"/>
-      <c r="R19" s="38"/>
-      <c r="S19" s="38"/>
-      <c r="T19" s="38"/>
-      <c r="U19" s="38"/>
-      <c r="V19" s="38"/>
-      <c r="W19" s="38"/>
-      <c r="X19" s="38"/>
-      <c r="Y19" s="38"/>
-      <c r="Z19" s="38"/>
+        <v>0.31580000000000003</v>
+      </c>
+      <c r="P19" s="13"/>
     </row>
     <row r="20" spans="1:26">
       <c r="A20" s="49">
         <f t="shared" si="2"/>
         <v>16</v>
       </c>
-      <c r="B20" s="13" t="s">
-        <v>104</v>
+      <c r="B20" s="18" t="s">
+        <v>108</v>
       </c>
       <c r="C20" s="13" t="s">
-        <v>180</v>
+        <v>197</v>
       </c>
       <c r="D20" s="18" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="E20" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="F20" s="18" t="s">
-        <v>106</v>
-      </c>
-      <c r="G20" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="F20" s="13"/>
+      <c r="G20" s="18" t="s">
         <v>107</v>
       </c>
       <c r="H20" s="18" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="I20" s="18" t="s">
         <v>9</v>
       </c>
       <c r="J20" s="18" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="K20" s="19">
-        <v>0.43</v>
+        <v>3.11</v>
       </c>
       <c r="L20" s="13">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="M20" s="51">
         <f t="shared" si="0"/>
-        <v>0.43</v>
+        <v>9.33</v>
       </c>
       <c r="N20" s="51">
-        <v>0.31580000000000003</v>
+        <v>2.4912000000000001</v>
       </c>
       <c r="O20" s="51">
         <f t="shared" si="1"/>
-        <v>0.31580000000000003</v>
+        <v>7.4736000000000002</v>
       </c>
       <c r="P20" s="13"/>
     </row>
@@ -2859,47 +2844,49 @@
         <f t="shared" si="2"/>
         <v>17</v>
       </c>
-      <c r="B21" s="18" t="s">
-        <v>111</v>
+      <c r="B21" s="13" t="s">
+        <v>112</v>
       </c>
       <c r="C21" s="13" t="s">
-        <v>207</v>
-      </c>
-      <c r="D21" s="18" t="s">
-        <v>112</v>
-      </c>
-      <c r="E21" s="18" t="s">
-        <v>24</v>
-      </c>
-      <c r="F21" s="13"/>
-      <c r="G21" s="18" t="s">
-        <v>110</v>
-      </c>
-      <c r="H21" s="18" t="s">
-        <v>113</v>
-      </c>
-      <c r="I21" s="18" t="s">
+        <v>187</v>
+      </c>
+      <c r="D21" s="21" t="s">
+        <v>97</v>
+      </c>
+      <c r="E21" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="F21" s="21" t="s">
+        <v>96</v>
+      </c>
+      <c r="G21" s="21" t="s">
+        <v>98</v>
+      </c>
+      <c r="H21" s="21" t="s">
+        <v>99</v>
+      </c>
+      <c r="I21" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="J21" s="18" t="s">
-        <v>114</v>
-      </c>
-      <c r="K21" s="19">
-        <v>3.11</v>
+      <c r="J21" s="21" t="s">
+        <v>100</v>
+      </c>
+      <c r="K21" s="27">
+        <v>0.56999999999999995</v>
       </c>
       <c r="L21" s="13">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="M21" s="51">
         <f t="shared" si="0"/>
-        <v>9.33</v>
+        <v>1.1399999999999999</v>
       </c>
       <c r="N21" s="51">
-        <v>2.4912000000000001</v>
+        <v>0.45500000000000002</v>
       </c>
       <c r="O21" s="51">
         <f t="shared" si="1"/>
-        <v>7.4736000000000002</v>
+        <v>0.91</v>
       </c>
       <c r="P21" s="13"/>
     </row>
@@ -2908,49 +2895,49 @@
         <f t="shared" si="2"/>
         <v>18</v>
       </c>
-      <c r="B22" s="13" t="s">
+      <c r="B22" s="18" t="s">
+        <v>113</v>
+      </c>
+      <c r="C22" s="13" t="s">
+        <v>173</v>
+      </c>
+      <c r="D22" s="18" t="s">
+        <v>114</v>
+      </c>
+      <c r="E22" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="F22" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="G22" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="H22" s="18" t="s">
         <v>115</v>
       </c>
-      <c r="C22" s="13" t="s">
-        <v>197</v>
-      </c>
-      <c r="D22" s="21" t="s">
-        <v>100</v>
-      </c>
-      <c r="E22" s="21" t="s">
-        <v>12</v>
-      </c>
-      <c r="F22" s="21" t="s">
-        <v>99</v>
-      </c>
-      <c r="G22" s="21" t="s">
-        <v>101</v>
-      </c>
-      <c r="H22" s="21" t="s">
-        <v>102</v>
-      </c>
-      <c r="I22" s="21" t="s">
+      <c r="I22" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="J22" s="21" t="s">
-        <v>103</v>
-      </c>
-      <c r="K22" s="27">
-        <v>0.56999999999999995</v>
+      <c r="J22" s="18" t="s">
+        <v>115</v>
+      </c>
+      <c r="K22" s="19">
+        <v>0.22</v>
       </c>
       <c r="L22" s="13">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M22" s="51">
         <f t="shared" si="0"/>
-        <v>1.1399999999999999</v>
+        <v>0.22</v>
       </c>
       <c r="N22" s="51">
-        <v>0.45500000000000002</v>
+        <v>0.1346</v>
       </c>
       <c r="O22" s="51">
         <f t="shared" si="1"/>
-        <v>0.91</v>
+        <v>0.1346</v>
       </c>
       <c r="P22" s="13"/>
     </row>
@@ -2959,49 +2946,49 @@
         <f t="shared" si="2"/>
         <v>19</v>
       </c>
-      <c r="B23" s="18" t="s">
-        <v>116</v>
+      <c r="B23" s="13" t="s">
+        <v>117</v>
       </c>
       <c r="C23" s="13" t="s">
-        <v>179</v>
+        <v>201</v>
       </c>
       <c r="D23" s="18" t="s">
-        <v>117</v>
-      </c>
-      <c r="E23" s="18" t="s">
+        <v>118</v>
+      </c>
+      <c r="E23" s="13" t="s">
         <v>12</v>
       </c>
       <c r="F23" s="18" t="s">
         <v>15</v>
       </c>
       <c r="G23" s="18" t="s">
-        <v>98</v>
+        <v>17</v>
       </c>
       <c r="H23" s="18" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="I23" s="18" t="s">
         <v>9</v>
       </c>
       <c r="J23" s="18" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="K23" s="19">
-        <v>0.22</v>
+        <v>5.8999999999999999E-3</v>
       </c>
       <c r="L23" s="13">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M23" s="51">
         <f t="shared" si="0"/>
-        <v>0.22</v>
+        <v>1.18E-2</v>
       </c>
       <c r="N23" s="51">
-        <v>0.1346</v>
+        <v>6.7999999999999996E-3</v>
       </c>
       <c r="O23" s="51">
         <f t="shared" si="1"/>
-        <v>0.1346</v>
+        <v>1.3599999999999999E-2</v>
       </c>
       <c r="P23" s="13"/>
     </row>
@@ -3011,15 +2998,15 @@
         <v>20</v>
       </c>
       <c r="B24" s="13" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C24" s="13" t="s">
-        <v>211</v>
+        <v>175</v>
       </c>
       <c r="D24" s="18" t="s">
-        <v>121</v>
-      </c>
-      <c r="E24" s="13" t="s">
+        <v>122</v>
+      </c>
+      <c r="E24" s="18" t="s">
         <v>12</v>
       </c>
       <c r="F24" s="18" t="s">
@@ -3029,30 +3016,30 @@
         <v>17</v>
       </c>
       <c r="H24" s="18" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="I24" s="18" t="s">
         <v>9</v>
       </c>
       <c r="J24" s="18" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="K24" s="19">
         <v>5.8999999999999999E-3</v>
       </c>
       <c r="L24" s="13">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="M24" s="51">
         <f t="shared" si="0"/>
-        <v>1.18E-2</v>
+        <v>2.3599999999999999E-2</v>
       </c>
       <c r="N24" s="51">
         <v>6.7999999999999996E-3</v>
       </c>
       <c r="O24" s="51">
         <f t="shared" si="1"/>
-        <v>1.3599999999999999E-2</v>
+        <v>2.7199999999999998E-2</v>
       </c>
       <c r="P24" s="13"/>
     </row>
@@ -3062,13 +3049,13 @@
         <v>21</v>
       </c>
       <c r="B25" s="13" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
       <c r="C25" s="13" t="s">
-        <v>181</v>
+        <v>228</v>
       </c>
       <c r="D25" s="18" t="s">
-        <v>125</v>
+        <v>30</v>
       </c>
       <c r="E25" s="18" t="s">
         <v>12</v>
@@ -3080,30 +3067,30 @@
         <v>17</v>
       </c>
       <c r="H25" s="18" t="s">
-        <v>126</v>
+        <v>31</v>
       </c>
       <c r="I25" s="18" t="s">
         <v>9</v>
       </c>
       <c r="J25" s="18" t="s">
-        <v>127</v>
+        <v>32</v>
       </c>
       <c r="K25" s="19">
         <v>5.8999999999999999E-3</v>
       </c>
       <c r="L25" s="13">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="M25" s="51">
         <f t="shared" si="0"/>
-        <v>2.3599999999999999E-2</v>
+        <v>3.5400000000000001E-2</v>
       </c>
       <c r="N25" s="51">
         <v>6.7999999999999996E-3</v>
       </c>
       <c r="O25" s="51">
         <f t="shared" si="1"/>
-        <v>2.7199999999999998E-2</v>
+        <v>4.0799999999999996E-2</v>
       </c>
       <c r="P25" s="13"/>
     </row>
@@ -3113,15 +3100,15 @@
         <v>22</v>
       </c>
       <c r="B26" s="13" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C26" s="13" t="s">
-        <v>243</v>
+        <v>202</v>
       </c>
       <c r="D26" s="18" t="s">
-        <v>30</v>
-      </c>
-      <c r="E26" s="18" t="s">
+        <v>131</v>
+      </c>
+      <c r="E26" s="13" t="s">
         <v>12</v>
       </c>
       <c r="F26" s="18" t="s">
@@ -3131,30 +3118,30 @@
         <v>17</v>
       </c>
       <c r="H26" s="18" t="s">
-        <v>31</v>
+        <v>132</v>
       </c>
       <c r="I26" s="18" t="s">
         <v>9</v>
       </c>
       <c r="J26" s="18" t="s">
-        <v>32</v>
+        <v>133</v>
       </c>
       <c r="K26" s="19">
         <v>5.8999999999999999E-3</v>
       </c>
       <c r="L26" s="13">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="M26" s="51">
         <f t="shared" si="0"/>
-        <v>3.5400000000000001E-2</v>
+        <v>2.3599999999999999E-2</v>
       </c>
       <c r="N26" s="51">
         <v>6.7999999999999996E-3</v>
       </c>
       <c r="O26" s="51">
         <f t="shared" si="1"/>
-        <v>4.0799999999999996E-2</v>
+        <v>2.7199999999999998E-2</v>
       </c>
       <c r="P26" s="13"/>
     </row>
@@ -3163,126 +3150,126 @@
         <f t="shared" si="2"/>
         <v>23</v>
       </c>
-      <c r="B27" s="13" t="s">
-        <v>133</v>
-      </c>
-      <c r="C27" s="13" t="s">
-        <v>212</v>
-      </c>
-      <c r="D27" s="18" t="s">
-        <v>134</v>
-      </c>
-      <c r="E27" s="13" t="s">
+      <c r="B27" s="32" t="s">
+        <v>125</v>
+      </c>
+      <c r="C27" s="32" t="s">
+        <v>199</v>
+      </c>
+      <c r="D27" s="33" t="s">
+        <v>126</v>
+      </c>
+      <c r="E27" s="33" t="s">
         <v>12</v>
       </c>
-      <c r="F27" s="18" t="s">
+      <c r="F27" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="G27" s="18" t="s">
+      <c r="G27" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="H27" s="18" t="s">
-        <v>135</v>
-      </c>
-      <c r="I27" s="18" t="s">
+      <c r="H27" s="33" t="s">
+        <v>127</v>
+      </c>
+      <c r="I27" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="J27" s="18" t="s">
-        <v>136</v>
-      </c>
-      <c r="K27" s="19">
+      <c r="J27" s="33" t="s">
+        <v>128</v>
+      </c>
+      <c r="K27" s="34">
         <v>5.8999999999999999E-3</v>
       </c>
-      <c r="L27" s="13">
-        <v>4</v>
+      <c r="L27" s="32">
+        <v>1</v>
       </c>
       <c r="M27" s="51">
         <f t="shared" si="0"/>
-        <v>2.3599999999999999E-2</v>
+        <v>5.8999999999999999E-3</v>
       </c>
       <c r="N27" s="51">
         <v>6.7999999999999996E-3</v>
       </c>
       <c r="O27" s="51">
         <f t="shared" si="1"/>
-        <v>2.7199999999999998E-2</v>
-      </c>
-      <c r="P27" s="13"/>
+        <v>6.7999999999999996E-3</v>
+      </c>
+      <c r="P27" s="32"/>
+      <c r="Q27" s="32"/>
+      <c r="R27" s="32"/>
+      <c r="S27" s="32"/>
+      <c r="T27" s="32"/>
+      <c r="U27" s="32"/>
+      <c r="V27" s="32"/>
+      <c r="W27" s="32"/>
+      <c r="X27" s="32"/>
+      <c r="Y27" s="32"/>
+      <c r="Z27" s="32"/>
     </row>
     <row r="28" spans="1:26">
       <c r="A28" s="49">
         <f t="shared" si="2"/>
         <v>24</v>
       </c>
-      <c r="B28" s="32" t="s">
-        <v>128</v>
-      </c>
-      <c r="C28" s="32" t="s">
-        <v>209</v>
-      </c>
-      <c r="D28" s="33" t="s">
-        <v>129</v>
-      </c>
-      <c r="E28" s="33" t="s">
+      <c r="B28" s="13" t="s">
+        <v>134</v>
+      </c>
+      <c r="C28" s="13" t="s">
+        <v>229</v>
+      </c>
+      <c r="D28" s="18" t="s">
+        <v>135</v>
+      </c>
+      <c r="E28" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="F28" s="33" t="s">
+      <c r="F28" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="G28" s="33" t="s">
+      <c r="G28" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="H28" s="33" t="s">
-        <v>130</v>
-      </c>
-      <c r="I28" s="33" t="s">
+      <c r="H28" s="18" t="s">
+        <v>136</v>
+      </c>
+      <c r="I28" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="J28" s="33" t="s">
-        <v>131</v>
-      </c>
-      <c r="K28" s="34">
+      <c r="J28" s="18" t="s">
+        <v>137</v>
+      </c>
+      <c r="K28" s="19">
         <v>5.8999999999999999E-3</v>
       </c>
-      <c r="L28" s="32">
-        <v>1</v>
+      <c r="L28" s="13">
+        <v>2</v>
       </c>
       <c r="M28" s="51">
         <f t="shared" si="0"/>
-        <v>5.8999999999999999E-3</v>
+        <v>1.18E-2</v>
       </c>
       <c r="N28" s="51">
         <v>6.7999999999999996E-3</v>
       </c>
       <c r="O28" s="51">
         <f t="shared" si="1"/>
-        <v>6.7999999999999996E-3</v>
-      </c>
-      <c r="P28" s="32"/>
-      <c r="Q28" s="32"/>
-      <c r="R28" s="32"/>
-      <c r="S28" s="32"/>
-      <c r="T28" s="32"/>
-      <c r="U28" s="32"/>
-      <c r="V28" s="32"/>
-      <c r="W28" s="32"/>
-      <c r="X28" s="32"/>
-      <c r="Y28" s="32"/>
-      <c r="Z28" s="32"/>
+        <v>1.3599999999999999E-2</v>
+      </c>
+      <c r="P28" s="13"/>
     </row>
     <row r="29" spans="1:26">
       <c r="A29" s="49">
         <f t="shared" si="2"/>
         <v>25</v>
       </c>
-      <c r="B29" s="13" t="s">
-        <v>137</v>
+      <c r="B29" s="18" t="s">
+        <v>139</v>
       </c>
       <c r="C29" s="13" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
       <c r="D29" s="18" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="E29" s="18" t="s">
         <v>12</v>
@@ -3291,26 +3278,26 @@
         <v>15</v>
       </c>
       <c r="G29" s="18" t="s">
-        <v>17</v>
+        <v>138</v>
       </c>
       <c r="H29" s="18" t="s">
-        <v>139</v>
-      </c>
-      <c r="I29" s="13" t="s">
+        <v>141</v>
+      </c>
+      <c r="I29" s="18" t="s">
         <v>9</v>
       </c>
       <c r="J29" s="18" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="K29" s="19">
-        <v>5.8999999999999999E-3</v>
+        <v>1.0999999999999999E-2</v>
       </c>
       <c r="L29" s="13">
         <v>2</v>
       </c>
       <c r="M29" s="51">
         <f t="shared" si="0"/>
-        <v>1.18E-2</v>
+        <v>2.1999999999999999E-2</v>
       </c>
       <c r="N29" s="51">
         <v>6.7999999999999996E-3</v>
@@ -3326,51 +3313,56 @@
         <f t="shared" si="2"/>
         <v>26</v>
       </c>
-      <c r="B30" s="18" t="s">
-        <v>142</v>
-      </c>
-      <c r="C30" s="13" t="s">
-        <v>183</v>
-      </c>
-      <c r="D30" s="18" t="s">
-        <v>143</v>
-      </c>
-      <c r="E30" s="18" t="s">
+      <c r="B30" s="57" t="s">
+        <v>223</v>
+      </c>
+      <c r="C30" s="57" t="s">
+        <v>212</v>
+      </c>
+      <c r="D30" s="58" t="s">
+        <v>224</v>
+      </c>
+      <c r="E30" s="58" t="s">
         <v>12</v>
       </c>
-      <c r="F30" s="18" t="s">
+      <c r="F30" s="58" t="s">
         <v>15</v>
       </c>
-      <c r="G30" s="18" t="s">
-        <v>141</v>
-      </c>
-      <c r="H30" s="18" t="s">
-        <v>144</v>
-      </c>
-      <c r="I30" s="18" t="s">
+      <c r="G30" s="58" t="s">
+        <v>138</v>
+      </c>
+      <c r="H30" s="58" t="s">
+        <v>225</v>
+      </c>
+      <c r="I30" s="57" t="s">
         <v>9</v>
       </c>
-      <c r="J30" s="18" t="s">
-        <v>145</v>
-      </c>
-      <c r="K30" s="19">
-        <v>1.0999999999999999E-2</v>
-      </c>
-      <c r="L30" s="13">
-        <v>2</v>
+      <c r="J30" s="58" t="s">
+        <v>226</v>
+      </c>
+      <c r="K30" s="59">
+        <v>1.1900000000000001E-2</v>
+      </c>
+      <c r="L30" s="57">
+        <v>100</v>
       </c>
       <c r="M30" s="51">
         <f t="shared" si="0"/>
-        <v>2.1999999999999999E-2</v>
-      </c>
-      <c r="N30" s="51">
-        <v>6.7999999999999996E-3</v>
-      </c>
-      <c r="O30" s="51">
-        <f t="shared" si="1"/>
-        <v>1.3599999999999999E-2</v>
-      </c>
-      <c r="P30" s="13"/>
+        <v>1.1900000000000002</v>
+      </c>
+      <c r="N30" s="57"/>
+      <c r="O30" s="57"/>
+      <c r="P30" s="57"/>
+      <c r="Q30" s="57"/>
+      <c r="R30" s="57"/>
+      <c r="S30" s="57"/>
+      <c r="T30" s="57"/>
+      <c r="U30" s="57"/>
+      <c r="V30" s="57"/>
+      <c r="W30" s="57"/>
+      <c r="X30" s="57"/>
+      <c r="Y30" s="57"/>
+      <c r="Z30" s="57"/>
     </row>
     <row r="31" spans="1:26">
       <c r="A31" s="49">
@@ -3378,13 +3370,13 @@
         <v>27</v>
       </c>
       <c r="B31" s="13" t="s">
-        <v>185</v>
+        <v>143</v>
       </c>
       <c r="C31" s="13" t="s">
-        <v>213</v>
-      </c>
-      <c r="D31" s="18" t="s">
-        <v>146</v>
+        <v>239</v>
+      </c>
+      <c r="D31" s="13" t="s">
+        <v>144</v>
       </c>
       <c r="E31" s="18" t="s">
         <v>12</v>
@@ -3392,34 +3384,34 @@
       <c r="F31" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="G31" s="18" t="s">
-        <v>141</v>
-      </c>
-      <c r="H31" s="18" t="s">
-        <v>147</v>
+      <c r="G31" s="13" t="s">
+        <v>116</v>
+      </c>
+      <c r="H31" s="13" t="s">
+        <v>145</v>
       </c>
       <c r="I31" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="J31" s="18" t="s">
-        <v>148</v>
+      <c r="J31" s="13" t="s">
+        <v>146</v>
       </c>
       <c r="K31" s="19">
-        <v>1.7500000000000002E-2</v>
+        <v>3.3099999999999997E-2</v>
       </c>
       <c r="L31" s="13">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="M31" s="51">
         <f t="shared" si="0"/>
-        <v>3.5000000000000003E-2</v>
+        <v>0.13239999999999999</v>
       </c>
       <c r="N31" s="51">
-        <v>6.7999999999999996E-3</v>
+        <v>3.4299999999999997E-2</v>
       </c>
       <c r="O31" s="51">
         <f t="shared" si="1"/>
-        <v>1.3599999999999999E-2</v>
+        <v>0.13719999999999999</v>
       </c>
       <c r="P31" s="13"/>
     </row>
@@ -3428,56 +3420,51 @@
         <f t="shared" si="2"/>
         <v>28</v>
       </c>
-      <c r="B32" s="57" t="s">
-        <v>238</v>
-      </c>
-      <c r="C32" s="57" t="s">
-        <v>223</v>
-      </c>
-      <c r="D32" s="58" t="s">
-        <v>239</v>
-      </c>
-      <c r="E32" s="58" t="s">
+      <c r="B32" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="C32" s="13" t="s">
+        <v>233</v>
+      </c>
+      <c r="D32" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="E32" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="F32" s="58" t="s">
+      <c r="F32" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="G32" s="58" t="s">
-        <v>141</v>
-      </c>
-      <c r="H32" s="58" t="s">
-        <v>240</v>
-      </c>
-      <c r="I32" s="57" t="s">
+      <c r="G32" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="H32" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="I32" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="J32" s="58" t="s">
-        <v>241</v>
-      </c>
-      <c r="K32" s="59">
-        <v>1.1900000000000001E-2</v>
-      </c>
-      <c r="L32" s="57">
-        <v>100</v>
+      <c r="J32" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="K32" s="19">
+        <v>0.1</v>
+      </c>
+      <c r="L32" s="13">
+        <v>4</v>
       </c>
       <c r="M32" s="51">
         <f t="shared" si="0"/>
-        <v>1.1900000000000002</v>
-      </c>
-      <c r="N32" s="57"/>
-      <c r="O32" s="57"/>
-      <c r="P32" s="57"/>
-      <c r="Q32" s="57"/>
-      <c r="R32" s="57"/>
-      <c r="S32" s="57"/>
-      <c r="T32" s="57"/>
-      <c r="U32" s="57"/>
-      <c r="V32" s="57"/>
-      <c r="W32" s="57"/>
-      <c r="X32" s="57"/>
-      <c r="Y32" s="57"/>
-      <c r="Z32" s="57"/>
+        <v>0.4</v>
+      </c>
+      <c r="N32" s="51">
+        <v>1.8499999999999999E-2</v>
+      </c>
+      <c r="O32" s="51">
+        <f t="shared" si="1"/>
+        <v>7.3999999999999996E-2</v>
+      </c>
+      <c r="P32" s="13"/>
     </row>
     <row r="33" spans="1:26">
       <c r="A33" s="49">
@@ -3485,48 +3472,48 @@
         <v>29</v>
       </c>
       <c r="B33" s="13" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C33" s="13" t="s">
-        <v>227</v>
-      </c>
-      <c r="D33" s="13" t="s">
-        <v>150</v>
-      </c>
-      <c r="E33" s="18" t="s">
+        <v>234</v>
+      </c>
+      <c r="D33" s="18" t="s">
+        <v>148</v>
+      </c>
+      <c r="E33" s="13" t="s">
         <v>12</v>
       </c>
       <c r="F33" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="G33" s="13" t="s">
-        <v>119</v>
-      </c>
-      <c r="H33" s="13" t="s">
-        <v>151</v>
+      <c r="G33" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="H33" s="18" t="s">
+        <v>149</v>
       </c>
       <c r="I33" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="J33" s="13" t="s">
-        <v>152</v>
+      <c r="J33" s="18" t="s">
+        <v>150</v>
       </c>
       <c r="K33" s="19">
-        <v>3.3099999999999997E-2</v>
+        <v>3.1600000000000003E-2</v>
       </c>
       <c r="L33" s="13">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="M33" s="51">
         <f t="shared" si="0"/>
-        <v>0.13239999999999999</v>
+        <v>0.18960000000000002</v>
       </c>
       <c r="N33" s="51">
-        <v>3.4299999999999997E-2</v>
+        <v>3.3099999999999997E-2</v>
       </c>
       <c r="O33" s="51">
         <f t="shared" si="1"/>
-        <v>0.13719999999999999</v>
+        <v>0.1986</v>
       </c>
       <c r="P33" s="13"/>
     </row>
@@ -3536,13 +3523,13 @@
         <v>30</v>
       </c>
       <c r="B34" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="C34" s="13" t="s">
-        <v>226</v>
-      </c>
-      <c r="D34" s="18" t="s">
-        <v>20</v>
+        <v>151</v>
+      </c>
+      <c r="C34" s="48" t="s">
+        <v>235</v>
+      </c>
+      <c r="D34" s="13" t="s">
+        <v>152</v>
       </c>
       <c r="E34" s="18" t="s">
         <v>12</v>
@@ -3553,31 +3540,31 @@
       <c r="G34" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="H34" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="I34" s="18" t="s">
+      <c r="H34" s="13" t="s">
+        <v>153</v>
+      </c>
+      <c r="I34" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="J34" s="18" t="s">
-        <v>22</v>
+      <c r="J34" s="13" t="s">
+        <v>154</v>
       </c>
       <c r="K34" s="19">
-        <v>0.1</v>
+        <v>4.3999999999999997E-2</v>
       </c>
       <c r="L34" s="13">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="M34" s="51">
         <f t="shared" si="0"/>
-        <v>0.4</v>
+        <v>8.7999999999999995E-2</v>
       </c>
       <c r="N34" s="51">
-        <v>1.8499999999999999E-2</v>
+        <v>4.48E-2</v>
       </c>
       <c r="O34" s="51">
         <f t="shared" si="1"/>
-        <v>7.3999999999999996E-2</v>
+        <v>8.9599999999999999E-2</v>
       </c>
       <c r="P34" s="13"/>
     </row>
@@ -3587,48 +3574,49 @@
         <v>31</v>
       </c>
       <c r="B35" s="13" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="C35" s="13" t="s">
-        <v>224</v>
+        <v>237</v>
       </c>
       <c r="D35" s="18" t="s">
-        <v>154</v>
-      </c>
-      <c r="E35" s="13" t="s">
+        <v>156</v>
+      </c>
+      <c r="E35" s="18" t="s">
         <v>12</v>
       </c>
       <c r="F35" s="18" t="s">
         <v>15</v>
       </c>
       <c r="G35" s="18" t="s">
-        <v>16</v>
+        <v>94</v>
       </c>
       <c r="H35" s="18" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="I35" s="18" t="s">
         <v>9</v>
       </c>
       <c r="J35" s="18" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="K35" s="19">
-        <v>3.1600000000000003E-2</v>
+        <v>6.3200000000000006E-2</v>
       </c>
       <c r="L35" s="13">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="M35" s="51">
         <f t="shared" si="0"/>
-        <v>0.18960000000000002</v>
+        <v>0.12640000000000001</v>
       </c>
       <c r="N35" s="51">
-        <v>3.3099999999999997E-2</v>
+        <f t="shared" si="0"/>
+        <v>0.25280000000000002</v>
       </c>
       <c r="O35" s="51">
         <f t="shared" si="1"/>
-        <v>0.1986</v>
+        <v>0.50560000000000005</v>
       </c>
       <c r="P35" s="13"/>
     </row>
@@ -3637,49 +3625,47 @@
         <f t="shared" si="2"/>
         <v>32</v>
       </c>
-      <c r="B36" s="13" t="s">
-        <v>157</v>
-      </c>
-      <c r="C36" s="13" t="s">
-        <v>184</v>
-      </c>
-      <c r="D36" s="13" t="s">
-        <v>158</v>
-      </c>
-      <c r="E36" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="F36" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="G36" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="H36" s="13" t="s">
+      <c r="B36" s="18" t="s">
         <v>159</v>
       </c>
-      <c r="I36" s="13" t="s">
+      <c r="D36" s="20" t="s">
+        <v>160</v>
+      </c>
+      <c r="E36" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="F36" s="28" t="s">
+        <v>70</v>
+      </c>
+      <c r="G36" s="20" t="s">
+        <v>161</v>
+      </c>
+      <c r="H36" s="20" t="s">
+        <v>162</v>
+      </c>
+      <c r="I36" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="J36" s="13" t="s">
-        <v>160</v>
-      </c>
-      <c r="K36" s="19">
-        <v>4.3999999999999997E-2</v>
+      <c r="J36" s="20" t="s">
+        <v>163</v>
+      </c>
+      <c r="K36" s="22">
+        <v>63.75</v>
       </c>
       <c r="L36" s="13">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M36" s="51">
         <f t="shared" si="0"/>
-        <v>8.7999999999999995E-2</v>
+        <v>63.75</v>
       </c>
       <c r="N36" s="51">
-        <v>4.48E-2</v>
+        <f t="shared" si="0"/>
+        <v>63.75</v>
       </c>
       <c r="O36" s="51">
         <f t="shared" si="1"/>
-        <v>8.9599999999999999E-2</v>
+        <v>63.75</v>
       </c>
       <c r="P36" s="13"/>
     </row>
@@ -3688,50 +3674,48 @@
         <f t="shared" si="2"/>
         <v>33</v>
       </c>
-      <c r="B37" s="13" t="s">
+      <c r="B37" s="18" t="s">
+        <v>164</v>
+      </c>
+      <c r="C37" s="13"/>
+      <c r="D37" s="20" t="s">
+        <v>165</v>
+      </c>
+      <c r="E37" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="F37" s="28" t="s">
+        <v>70</v>
+      </c>
+      <c r="G37" s="20" t="s">
         <v>161</v>
       </c>
-      <c r="C37" s="13" t="s">
-        <v>182</v>
-      </c>
-      <c r="D37" s="18" t="s">
-        <v>162</v>
-      </c>
-      <c r="E37" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="F37" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="G37" s="18" t="s">
-        <v>97</v>
-      </c>
-      <c r="H37" s="18" t="s">
-        <v>163</v>
-      </c>
-      <c r="I37" s="18" t="s">
+      <c r="H37" s="20" t="s">
+        <v>166</v>
+      </c>
+      <c r="I37" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="J37" s="18" t="s">
-        <v>164</v>
-      </c>
-      <c r="K37" s="19">
-        <v>6.3200000000000006E-2</v>
+      <c r="J37" s="20" t="s">
+        <v>167</v>
+      </c>
+      <c r="K37" s="22">
+        <v>31.88</v>
       </c>
       <c r="L37" s="13">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M37" s="51">
         <f t="shared" si="0"/>
-        <v>0.12640000000000001</v>
+        <v>31.88</v>
       </c>
       <c r="N37" s="51">
         <f t="shared" si="0"/>
-        <v>0.25280000000000002</v>
+        <v>31.88</v>
       </c>
       <c r="O37" s="51">
         <f t="shared" si="1"/>
-        <v>0.50560000000000005</v>
+        <v>31.88</v>
       </c>
       <c r="P37" s="13"/>
     </row>
@@ -3740,331 +3724,287 @@
         <f t="shared" si="2"/>
         <v>34</v>
       </c>
-      <c r="B38" s="18" t="s">
-        <v>165</v>
-      </c>
-      <c r="D38" s="20" t="s">
-        <v>166</v>
-      </c>
-      <c r="E38" s="21" t="s">
-        <v>73</v>
-      </c>
-      <c r="F38" s="28" t="s">
-        <v>73</v>
-      </c>
-      <c r="G38" s="20" t="s">
-        <v>167</v>
-      </c>
-      <c r="H38" s="20" t="s">
-        <v>168</v>
-      </c>
-      <c r="I38" s="21" t="s">
+      <c r="B38" s="45" t="s">
+        <v>205</v>
+      </c>
+      <c r="C38" s="45" t="s">
+        <v>196</v>
+      </c>
+      <c r="D38" s="45" t="s">
+        <v>206</v>
+      </c>
+      <c r="E38" s="45" t="s">
+        <v>12</v>
+      </c>
+      <c r="F38" s="46" t="s">
+        <v>15</v>
+      </c>
+      <c r="G38" s="45" t="s">
+        <v>116</v>
+      </c>
+      <c r="H38" s="45" t="s">
+        <v>207</v>
+      </c>
+      <c r="I38" s="46" t="s">
         <v>9</v>
       </c>
-      <c r="J38" s="20" t="s">
-        <v>169</v>
-      </c>
-      <c r="K38" s="22">
-        <v>63.75</v>
-      </c>
-      <c r="L38" s="13">
+      <c r="J38" s="45" t="s">
+        <v>208</v>
+      </c>
+      <c r="K38" s="47">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="L38" s="45">
         <v>1</v>
       </c>
       <c r="M38" s="51">
         <f t="shared" si="0"/>
-        <v>63.75</v>
+        <v>7.0000000000000001E-3</v>
       </c>
       <c r="N38" s="51">
-        <f t="shared" si="0"/>
-        <v>63.75</v>
+        <v>7.0000000000000001E-3</v>
       </c>
       <c r="O38" s="51">
         <f t="shared" si="1"/>
-        <v>63.75</v>
-      </c>
-      <c r="P38" s="13"/>
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="P38" s="45"/>
+      <c r="Q38" s="45"/>
+      <c r="R38" s="45"/>
+      <c r="S38" s="45"/>
+      <c r="T38" s="45"/>
+      <c r="U38" s="45"/>
+      <c r="V38" s="45"/>
+      <c r="W38" s="45"/>
+      <c r="X38" s="45"/>
+      <c r="Y38" s="45"/>
+      <c r="Z38" s="45"/>
     </row>
     <row r="39" spans="1:26">
       <c r="A39" s="49">
         <f t="shared" si="2"/>
         <v>35</v>
       </c>
-      <c r="B39" s="18" t="s">
-        <v>170</v>
-      </c>
-      <c r="C39" s="13"/>
-      <c r="D39" s="20" t="s">
-        <v>171</v>
-      </c>
-      <c r="E39" s="21" t="s">
-        <v>73</v>
-      </c>
-      <c r="F39" s="28" t="s">
-        <v>73</v>
-      </c>
-      <c r="G39" s="20" t="s">
-        <v>167</v>
-      </c>
-      <c r="H39" s="20" t="s">
-        <v>172</v>
-      </c>
-      <c r="I39" s="21" t="s">
+      <c r="B39" s="48" t="s">
+        <v>19</v>
+      </c>
+      <c r="C39" s="50" t="s">
+        <v>198</v>
+      </c>
+      <c r="D39" s="50" t="s">
+        <v>25</v>
+      </c>
+      <c r="E39" s="50" t="s">
+        <v>24</v>
+      </c>
+      <c r="F39" s="50"/>
+      <c r="G39" s="50" t="s">
+        <v>26</v>
+      </c>
+      <c r="H39" s="50" t="s">
+        <v>27</v>
+      </c>
+      <c r="I39" s="50" t="s">
         <v>9</v>
       </c>
-      <c r="J39" s="20" t="s">
-        <v>173</v>
-      </c>
-      <c r="K39" s="22">
-        <v>31.88</v>
-      </c>
-      <c r="L39" s="13">
+      <c r="J39" s="50" t="s">
+        <v>28</v>
+      </c>
+      <c r="K39" s="51">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="L39" s="48">
         <v>1</v>
       </c>
       <c r="M39" s="51">
         <f t="shared" si="0"/>
-        <v>31.88</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="N39" s="51">
-        <f t="shared" si="0"/>
-        <v>31.88</v>
+        <v>0.3982</v>
       </c>
       <c r="O39" s="51">
         <f t="shared" si="1"/>
-        <v>31.88</v>
-      </c>
-      <c r="P39" s="13"/>
-    </row>
-    <row r="40" spans="1:26">
+        <v>0.3982</v>
+      </c>
+      <c r="P39" s="48"/>
+      <c r="Q39" s="48"/>
+      <c r="R39" s="48"/>
+      <c r="S39" s="48"/>
+      <c r="T39" s="48"/>
+      <c r="U39" s="48"/>
+      <c r="V39" s="48"/>
+      <c r="W39" s="48"/>
+      <c r="X39" s="48"/>
+      <c r="Y39" s="48"/>
+      <c r="Z39" s="48"/>
+    </row>
+    <row r="40" spans="1:26" ht="12">
       <c r="A40" s="49">
         <f t="shared" si="2"/>
         <v>36</v>
       </c>
-      <c r="B40" s="45" t="s">
-        <v>216</v>
-      </c>
-      <c r="C40" s="45" t="s">
-        <v>206</v>
-      </c>
-      <c r="D40" s="45" t="s">
-        <v>217</v>
-      </c>
-      <c r="E40" s="45" t="s">
+      <c r="B40" s="13" t="s">
+        <v>200</v>
+      </c>
+      <c r="C40" s="13" t="s">
+        <v>236</v>
+      </c>
+      <c r="D40" s="48" t="s">
+        <v>219</v>
+      </c>
+      <c r="E40" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="F40" s="46" t="s">
+      <c r="F40" s="50" t="s">
         <v>15</v>
       </c>
-      <c r="G40" s="45" t="s">
-        <v>119</v>
-      </c>
-      <c r="H40" s="45" t="s">
-        <v>218</v>
-      </c>
-      <c r="I40" s="46" t="s">
+      <c r="G40" s="48" t="s">
+        <v>16</v>
+      </c>
+      <c r="H40" s="48" t="s">
+        <v>220</v>
+      </c>
+      <c r="I40" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="J40" s="45" t="s">
-        <v>219</v>
-      </c>
-      <c r="K40" s="47">
-        <v>7.0000000000000001E-3</v>
-      </c>
-      <c r="L40" s="45">
+      <c r="J40" s="52" t="s">
+        <v>221</v>
+      </c>
+      <c r="K40" s="13">
+        <v>0.1</v>
+      </c>
+      <c r="L40" s="13">
         <v>1</v>
       </c>
       <c r="M40" s="51">
         <f t="shared" si="0"/>
-        <v>7.0000000000000001E-3</v>
-      </c>
-      <c r="N40" s="51">
-        <v>7.0000000000000001E-3</v>
+        <v>0.1</v>
+      </c>
+      <c r="N40" s="56">
+        <v>1.6299999999999999E-2</v>
       </c>
       <c r="O40" s="51">
         <f t="shared" si="1"/>
-        <v>7.0000000000000001E-3</v>
-      </c>
-      <c r="P40" s="45"/>
-      <c r="Q40" s="45"/>
-      <c r="R40" s="45"/>
-      <c r="S40" s="45"/>
-      <c r="T40" s="45"/>
-      <c r="U40" s="45"/>
-      <c r="V40" s="45"/>
-      <c r="W40" s="45"/>
-      <c r="X40" s="45"/>
-      <c r="Y40" s="45"/>
-      <c r="Z40" s="45"/>
+        <v>1.6299999999999999E-2</v>
+      </c>
+      <c r="P40" s="14"/>
     </row>
     <row r="41" spans="1:26">
       <c r="A41" s="49">
         <f t="shared" si="2"/>
         <v>37</v>
       </c>
-      <c r="B41" s="48" t="s">
-        <v>19</v>
-      </c>
-      <c r="C41" s="50" t="s">
-        <v>208</v>
-      </c>
-      <c r="D41" s="50" t="s">
-        <v>25</v>
-      </c>
-      <c r="E41" s="50" t="s">
-        <v>24</v>
-      </c>
-      <c r="F41" s="50"/>
-      <c r="G41" s="50" t="s">
-        <v>26</v>
-      </c>
-      <c r="H41" s="50" t="s">
-        <v>27</v>
+      <c r="B41" s="41" t="s">
+        <v>101</v>
+      </c>
+      <c r="C41" s="41" t="s">
+        <v>204</v>
+      </c>
+      <c r="D41" s="42" t="s">
+        <v>102</v>
+      </c>
+      <c r="E41" s="42" t="s">
+        <v>12</v>
+      </c>
+      <c r="F41" s="42" t="s">
+        <v>103</v>
+      </c>
+      <c r="G41" s="44" t="s">
+        <v>104</v>
+      </c>
+      <c r="H41" s="42" t="s">
+        <v>105</v>
       </c>
       <c r="I41" s="50" t="s">
         <v>9</v>
       </c>
-      <c r="J41" s="50" t="s">
-        <v>28</v>
-      </c>
-      <c r="K41" s="51">
-        <v>0.55000000000000004</v>
-      </c>
-      <c r="L41" s="48">
+      <c r="J41" s="42" t="s">
+        <v>106</v>
+      </c>
+      <c r="K41" s="43">
+        <v>0.43</v>
+      </c>
+      <c r="L41" s="41">
         <v>1</v>
       </c>
       <c r="M41" s="51">
         <f t="shared" si="0"/>
-        <v>0.55000000000000004</v>
+        <v>0.43</v>
       </c>
       <c r="N41" s="51">
-        <v>0.3982</v>
+        <v>0.31580000000000003</v>
       </c>
       <c r="O41" s="51">
         <f t="shared" si="1"/>
-        <v>0.3982</v>
-      </c>
-      <c r="P41" s="48"/>
-      <c r="Q41" s="48"/>
-      <c r="R41" s="48"/>
-      <c r="S41" s="48"/>
-      <c r="T41" s="48"/>
-      <c r="U41" s="48"/>
-      <c r="V41" s="48"/>
-      <c r="W41" s="48"/>
-      <c r="X41" s="48"/>
-      <c r="Y41" s="48"/>
-      <c r="Z41" s="48"/>
-    </row>
-    <row r="42" spans="1:26" ht="12">
+        <v>0.31580000000000003</v>
+      </c>
+      <c r="P41" s="41"/>
+      <c r="Q41" s="41"/>
+      <c r="R41" s="41"/>
+      <c r="S41" s="41"/>
+      <c r="T41" s="41"/>
+      <c r="U41" s="41"/>
+      <c r="V41" s="41"/>
+      <c r="W41" s="41"/>
+      <c r="X41" s="41"/>
+      <c r="Y41" s="41"/>
+      <c r="Z41" s="41"/>
+    </row>
+    <row r="42" spans="1:26">
       <c r="A42" s="49">
         <f t="shared" si="2"/>
         <v>38</v>
       </c>
-      <c r="B42" s="13" t="s">
-        <v>210</v>
-      </c>
-      <c r="C42" s="13" t="s">
-        <v>225</v>
-      </c>
-      <c r="D42" s="48" t="s">
-        <v>234</v>
-      </c>
-      <c r="E42" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="F42" s="50" t="s">
-        <v>15</v>
-      </c>
-      <c r="G42" s="48" t="s">
-        <v>16</v>
-      </c>
-      <c r="H42" s="48" t="s">
-        <v>235</v>
-      </c>
-      <c r="I42" s="13" t="s">
+      <c r="B42" s="63" t="s">
+        <v>58</v>
+      </c>
+      <c r="C42" s="63" t="s">
+        <v>180</v>
+      </c>
+      <c r="D42" s="65" t="s">
+        <v>230</v>
+      </c>
+      <c r="E42" s="65" t="s">
+        <v>59</v>
+      </c>
+      <c r="F42" s="65" t="s">
+        <v>60</v>
+      </c>
+      <c r="G42" s="65" t="s">
+        <v>61</v>
+      </c>
+      <c r="H42" s="65" t="s">
+        <v>231</v>
+      </c>
+      <c r="I42" s="66" t="s">
         <v>9</v>
       </c>
-      <c r="J42" s="52" t="s">
-        <v>236</v>
-      </c>
-      <c r="K42" s="13">
-        <v>0.1</v>
-      </c>
-      <c r="L42" s="13">
-        <v>1</v>
-      </c>
-      <c r="M42" s="51">
-        <f t="shared" si="0"/>
-        <v>0.1</v>
-      </c>
-      <c r="N42" s="56">
-        <v>1.6299999999999999E-2</v>
-      </c>
-      <c r="O42" s="51">
-        <f t="shared" si="1"/>
-        <v>1.6299999999999999E-2</v>
-      </c>
-      <c r="P42" s="14"/>
-    </row>
-    <row r="43" spans="1:26">
-      <c r="A43" s="49">
-        <f t="shared" si="2"/>
-        <v>39</v>
-      </c>
-      <c r="B43" s="41" t="s">
-        <v>104</v>
-      </c>
-      <c r="C43" s="41" t="s">
-        <v>215</v>
-      </c>
-      <c r="D43" s="42" t="s">
-        <v>105</v>
-      </c>
-      <c r="E43" s="42" t="s">
-        <v>12</v>
-      </c>
-      <c r="F43" s="42" t="s">
-        <v>106</v>
-      </c>
-      <c r="G43" s="44" t="s">
-        <v>107</v>
-      </c>
-      <c r="H43" s="42" t="s">
-        <v>108</v>
-      </c>
-      <c r="I43" s="50" t="s">
-        <v>9</v>
-      </c>
-      <c r="J43" s="42" t="s">
-        <v>109</v>
-      </c>
-      <c r="K43" s="43">
-        <v>0.43</v>
-      </c>
-      <c r="L43" s="41">
-        <v>1</v>
-      </c>
-      <c r="M43" s="51">
-        <f t="shared" si="0"/>
-        <v>0.43</v>
-      </c>
-      <c r="N43" s="51">
-        <v>0.31580000000000003</v>
-      </c>
-      <c r="O43" s="51">
-        <f t="shared" si="1"/>
-        <v>0.31580000000000003</v>
-      </c>
-      <c r="P43" s="41"/>
-      <c r="Q43" s="41"/>
-      <c r="R43" s="41"/>
-      <c r="S43" s="41"/>
-      <c r="T43" s="41"/>
-      <c r="U43" s="41"/>
-      <c r="V43" s="41"/>
-      <c r="W43" s="41"/>
-      <c r="X43" s="41"/>
-      <c r="Y43" s="41"/>
-      <c r="Z43" s="41"/>
+      <c r="J42" s="65" t="s">
+        <v>232</v>
+      </c>
+      <c r="K42" s="67">
+        <v>5.95</v>
+      </c>
+      <c r="L42" s="63">
+        <v>3</v>
+      </c>
+      <c r="M42" s="64">
+        <v>17.850000000000001</v>
+      </c>
+      <c r="N42" s="63"/>
+      <c r="O42" s="63"/>
+      <c r="P42" s="63"/>
+      <c r="Q42" s="63"/>
+      <c r="R42" s="63"/>
+      <c r="S42" s="63"/>
+      <c r="T42" s="63"/>
+      <c r="U42" s="63"/>
+      <c r="V42" s="63"/>
+      <c r="W42" s="63"/>
+      <c r="X42" s="63"/>
+      <c r="Y42" s="63"/>
+      <c r="Z42" s="63"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>